<commit_message>
added pages & tests
</commit_message>
<xml_diff>
--- a/target/classes/com/crm/qa/testdata/freeCrmTestData.xlsx
+++ b/target/classes/com/crm/qa/testdata/freeCrmTestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Companies" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>title</t>
   </si>
@@ -64,6 +64,126 @@
   </si>
   <si>
     <t>Swapnali</t>
+  </si>
+  <si>
+    <t>compName</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>employees</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Inactive</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Ad</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Thane</t>
+  </si>
+  <si>
+    <t>Mumbai address</t>
+  </si>
+  <si>
+    <t>Thane address</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>400028</t>
+  </si>
+  <si>
+    <t>3000000</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>400063</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>FMCG</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>140000000</t>
   </si>
 </sst>
 </file>
@@ -105,9 +225,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,12 +601,163 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>